<commit_message>
webpack seems to mess up loading my rollup google lib, gapi does not work properly
</commit_message>
<xml_diff>
--- a/libs/accounts/src/test/example_xlsx/Account-Assets.xlsx
+++ b/libs/accounts/src/test/example_xlsx/Account-Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aultac/repos/aultfarms/af-monorepo/libs/accounts/src/test/example_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B20399-33A0-DD40-9A7B-415DA64F002F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED422FAC-3942-C342-AA81-1E4473ADD19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1400" windowWidth="35840" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="1320" windowWidth="35840" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equipmentauto.2020" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Added ability to export an account, fixed MAJOR bug in how split dates got filled in (now the parent properly filled in written/post)
</commit_message>
<xml_diff>
--- a/libs/accounts/src/test/example_xlsx/Account-Assets.xlsx
+++ b/libs/accounts/src/test/example_xlsx/Account-Assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aultac/repos/aultfarms/af-monorepo/libs/accounts/src/test/example_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED422FAC-3942-C342-AA81-1E4473ADD19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DFFC33-D80D-D34F-9CE2-A85A5360BA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1320" windowWidth="35840" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1320" windowWidth="35840" windowHeight="12340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equipmentauto.2020" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="bldg_imprv.2020" sheetId="3" r:id="rId3"/>
     <sheet name="coop-test" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -668,8 +668,8 @@
   </sheetPr>
   <dimension ref="A1:AN875"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
@@ -30305,11 +30305,11 @@
   </sheetPr>
   <dimension ref="A1:AN899"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30445,8 +30445,12 @@
         <f>SUM(Q4:Q898)</f>
         <v>10000</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="6"/>
+      <c r="R3" s="5">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:40" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">

</xml_diff>